<commit_message>
Tableaux d'armes au complet
</commit_message>
<xml_diff>
--- a/Armes et protection.xlsx
+++ b/Armes et protection.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="116" documentId="11_F25DC773A252ABEACE02EC973B5B5D0C5ADE589F" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{4BAF3D2D-B2A5-4B54-85BC-2D7A2CE51F79}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3EB144-97F7-4960-B196-0ABADD7BCC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Armes à distance" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="99">
   <si>
     <t>Type</t>
   </si>
@@ -160,13 +160,172 @@
   </si>
   <si>
     <t>*** Recharger une arbalète prend 3 tours</t>
+  </si>
+  <si>
+    <t>Matraque</t>
+  </si>
+  <si>
+    <t>Particularités</t>
+  </si>
+  <si>
+    <t>Poing américain</t>
+  </si>
+  <si>
+    <t>Tonfa de police</t>
+  </si>
+  <si>
+    <t>Pied-de-biche</t>
+  </si>
+  <si>
+    <t>Démonte-pneu</t>
+  </si>
+  <si>
+    <t>Chaîne</t>
+  </si>
+  <si>
+    <t>Bouclier (petit)</t>
+  </si>
+  <si>
+    <t>Bouclier (grand)</t>
+  </si>
+  <si>
+    <t>Couteau</t>
+  </si>
+  <si>
+    <t>Rapière</t>
+  </si>
+  <si>
+    <t>Machette</t>
+  </si>
+  <si>
+    <t>Hachette</t>
+  </si>
+  <si>
+    <t>Hache anti-incendie</t>
+  </si>
+  <si>
+    <t>Tronçonneuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pieu * </t>
+  </si>
+  <si>
+    <t>Lance **</t>
+  </si>
+  <si>
+    <t>•</t>
+  </si>
+  <si>
+    <t>S/O</t>
+  </si>
+  <si>
+    <t>Étourdissant</t>
+  </si>
+  <si>
+    <t>Se manie avec Bagarre</t>
+  </si>
+  <si>
+    <t>Lutte</t>
+  </si>
+  <si>
+    <t>Protection</t>
+  </si>
+  <si>
+    <t>Perforant 1</t>
+  </si>
+  <si>
+    <t>9-relance, deux mains</t>
+  </si>
+  <si>
+    <t>Défense + 1, deux mains</t>
+  </si>
+  <si>
+    <t>Défense + 1</t>
+  </si>
+  <si>
+    <t>Défense</t>
+  </si>
+  <si>
+    <t>Vitesse</t>
+  </si>
+  <si>
+    <t>Parties protégées</t>
+  </si>
+  <si>
+    <t>MODERNES</t>
+  </si>
+  <si>
+    <t>Vêtements renforcés *</t>
+  </si>
+  <si>
+    <t>Veste en kevlar *</t>
+  </si>
+  <si>
+    <t>Veste pare-balles</t>
+  </si>
+  <si>
+    <t>Tenue antiémeute</t>
+  </si>
+  <si>
+    <t>Cuir (renforcé)</t>
+  </si>
+  <si>
+    <t>Cotte de mailles</t>
+  </si>
+  <si>
+    <t>Plate</t>
+  </si>
+  <si>
+    <t>ARCHAÏQUES</t>
+  </si>
+  <si>
+    <t>1/0</t>
+  </si>
+  <si>
+    <t>1/3</t>
+  </si>
+  <si>
+    <t>2/4</t>
+  </si>
+  <si>
+    <t>3/5</t>
+  </si>
+  <si>
+    <t>2/0</t>
+  </si>
+  <si>
+    <t>3/1</t>
+  </si>
+  <si>
+    <t>4/2</t>
+  </si>
+  <si>
+    <t>••••</t>
+  </si>
+  <si>
+    <t>Torse, bras, jambes</t>
+  </si>
+  <si>
+    <t>Torse</t>
+  </si>
+  <si>
+    <t>Torse, bras</t>
+  </si>
+  <si>
+    <t>* cette protection peut passer inaperçue</t>
+  </si>
+  <si>
+    <t>* Tenter de perçer le coeur de son adversaire a un malus de -3 et doit obtenir 5 réussites</t>
+  </si>
+  <si>
+    <t>** L'allonge de la lance fournit un bonus de +1 en Défense contre les adversaires désarmés ou munis d'une arme de Taille 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +338,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,11 +368,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,54 +663,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -565,7 +739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -594,7 +768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -623,7 +797,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -652,7 +826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -681,7 +855,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -710,7 +884,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -739,7 +913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -768,7 +942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -797,7 +971,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -823,17 +997,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -846,26 +1020,651 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47072CE3-15D2-49C8-AF1A-F95E6D09C02C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>-2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>-3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>-3</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>-2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>-4</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>-2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>-2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>-2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>-4</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>-6</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>-4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>-2</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164357A0-4CE4-444C-9E8C-0E5DC60FE2DF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>-2</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>-2</v>
+      </c>
+      <c r="E9">
+        <v>-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>-2</v>
+      </c>
+      <c r="E10">
+        <v>-3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A7:G7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>